<commit_message>
moddules and packages completed
</commit_message>
<xml_diff>
--- a/PythonRoadMap.xlsx
+++ b/PythonRoadMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravikantpal/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Jupyter_world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CFA496-C821-A647-9081-7D942C8D7A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1473636-D649-4131-AA45-181C4996BC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1606A581-AF28-FA4B-9F7F-5ED69F543647}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1606A581-AF28-FA4B-9F7F-5ED69F543647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Phase/Week</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Install Python, VS Code, Git</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>This one is done </t>
@@ -321,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -361,7 +358,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -467,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,7 +606,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,19 +617,19 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -660,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>45882</v>
@@ -669,18 +666,18 @@
         <v>45888</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D3" s="5">
         <v>45884</v>
@@ -689,18 +686,18 @@
         <v>45890</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3">
         <v>45886</v>
@@ -710,15 +707,15 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <v>45888</v>
@@ -728,15 +725,15 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5">
         <v>45890</v>
@@ -746,15 +743,15 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3">
         <v>45892</v>
@@ -764,15 +761,15 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <v>45894</v>
@@ -782,15 +779,15 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3">
         <v>45896</v>
@@ -800,15 +797,15 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3">
         <v>45898</v>
@@ -818,15 +815,15 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3">
         <v>45900</v>
@@ -836,15 +833,15 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3">
         <v>45902</v>
@@ -854,15 +851,15 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3">
         <v>45904</v>
@@ -872,15 +869,15 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3">
         <v>45906</v>
@@ -890,15 +887,15 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="3">
         <v>45908</v>
@@ -908,15 +905,15 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3">
         <v>45910</v>
@@ -926,15 +923,15 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3">
         <v>45912</v>
@@ -944,15 +941,15 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="3">
         <v>45914</v>
@@ -962,15 +959,15 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3">
         <v>45916</v>
@@ -980,15 +977,15 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3">
         <v>45918</v>
@@ -998,15 +995,15 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="3">
         <v>45920</v>
@@ -1016,15 +1013,15 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="3">
         <v>45922</v>
@@ -1034,15 +1031,15 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3">
         <v>45924</v>
@@ -1052,15 +1049,15 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3">
         <v>45926</v>
@@ -1082,7 +1079,7 @@
       <formula>$C2="To Do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24" xr:uid="{432A0C83-3551-694F-A277-CE3D32BE30D5}">
       <formula1>"To Do,In Progress,Done"</formula1>
     </dataValidation>

</xml_diff>